<commit_message>
li and la resources in CNT
</commit_message>
<xml_diff>
--- a/testes.xlsx
+++ b/testes.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelpereira/Library/Mobile Documents/com~apple~CloudDocs/Projetos/Mestrado/MobilidadeComputacional/Tiny-OneM2M-C-Language/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelpereira/Library/Mobile Documents/com~apple~CloudDocs/Projetos/Mestrado/MobilidadeComputacional/Aux/Tiny-OneM2M-C-Language/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{118CF29B-953A-AC42-B1ED-CF13A71410D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F0CD78-46D4-1643-8F09-CAFEC6761A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Machines" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="POST CIN" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>POST</t>
   </si>
@@ -199,12 +200,38 @@
 Avg: 1.257258
 Std Dev: 0.008587</t>
   </si>
+  <si>
+    <t>Raspi 0 W</t>
+  </si>
+  <si>
+    <t>HomePC</t>
+  </si>
+  <si>
+    <t>Dado este CNT</t>
+  </si>
+  <si>
+    <t>Calculating stats for POST
+Min: 0.145584
+Max: 0.231254
+Avg: 0.173087
+Std Dev: 0.016045</t>
+  </si>
+  <si>
+    <t>Obteve-se este resultado</t>
+  </si>
+  <si>
+    <t>Calculating stats for POST
+Min: 0.166321
+Max: 0.409225
+Avg: 0.213821
+Std Dev: 0.027584</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +244,25 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -246,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -267,12 +313,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -288,6 +339,331 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>121908</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB7CE557-BA82-41F8-EF61-3F770371DF04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="825500" y="381000"/>
+          <a:ext cx="8267700" cy="5455908"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>379452</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A589E94-ADB8-DF2E-9ADA-9A1CA1358E52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9118600" y="393700"/>
+          <a:ext cx="6945352" cy="5473700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>812801</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>35099</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{811E2405-75E5-D6CF-21B9-6FFC869BF73C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="825501" y="6286500"/>
+          <a:ext cx="8242300" cy="4988099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>37151</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D4CEDEC-0644-852D-0EEB-D8975764D110}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9055100" y="6299200"/>
+          <a:ext cx="6845300" cy="4977451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7060343F-4B37-9BF2-D89E-B0302F431B20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1689100" y="584200"/>
+          <a:ext cx="3657600" cy="2476500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A340CB4D-59A5-FB82-B1D3-6D857C978824}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1651000" y="3314700"/>
+          <a:ext cx="3657600" cy="2476500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -587,13 +963,85 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF8DCEC-D018-5640-9883-BCA0549E0527}">
+  <dimension ref="B1:K33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B32" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:K2"/>
+    <mergeCell ref="B32:K33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="B1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="200" workbookViewId="0">
+    <sheetView zoomScale="75" workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -632,12 +1080,12 @@
       </c>
     </row>
     <row r="4" spans="2:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="2:13" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
@@ -739,12 +1187,12 @@
     </row>
     <row r="9" spans="2:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="2:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="2:13" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
@@ -787,7 +1235,7 @@
       <c r="B13" s="6">
         <v>1000</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>20</v>
       </c>
       <c r="H13" s="6">
@@ -801,7 +1249,7 @@
       <c r="B14" s="6">
         <v>2000</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -867,4 +1315,77 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6745B2-8E6C-F04C-A1E2-2918CE09E162}">
+  <dimension ref="B1:K30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="19.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C3" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H4" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="81" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="96" x14ac:dyDescent="0.2">
+      <c r="H16" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:K2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>